<commit_message>
updated fan calculations for thermal management
</commit_message>
<xml_diff>
--- a/CamperVan.xlsx
+++ b/CamperVan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adrian/Documents/Campervan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20FBC8C-AA4E-A84A-A1FF-3A43CF3966A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB07540-5D3D-A641-8CFB-E60E766882A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="21360" activeTab="8" xr2:uid="{32DB9825-7707-5644-AF59-E2F85CFFFB5B}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="21360" activeTab="10" xr2:uid="{32DB9825-7707-5644-AF59-E2F85CFFFB5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="Resistor" sheetId="11" r:id="rId8"/>
     <sheet name="Cable" sheetId="12" r:id="rId9"/>
     <sheet name="Tanks" sheetId="10" r:id="rId10"/>
+    <sheet name="Fans" sheetId="13" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="336">
   <si>
     <t>Item</t>
   </si>
@@ -990,14 +991,102 @@
   <si>
     <t>Voltage Drop</t>
   </si>
+  <si>
+    <t>m^3/min</t>
+  </si>
+  <si>
+    <t>50A DC-DC convertor</t>
+  </si>
+  <si>
+    <t>Wattage</t>
+  </si>
+  <si>
+    <t>Q' = W/20deltaT</t>
+  </si>
+  <si>
+    <t>delta T</t>
+  </si>
+  <si>
+    <t>Q'</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>Q (2*Q')</t>
+  </si>
+  <si>
+    <t>200Ah Battery</t>
+  </si>
+  <si>
+    <t>Q (1.5*Q')</t>
+  </si>
+  <si>
+    <t>Output Power</t>
+  </si>
+  <si>
+    <t>Efficiency</t>
+  </si>
+  <si>
+    <t>Input Power</t>
+  </si>
+  <si>
+    <t>Power Dissipation</t>
+  </si>
+  <si>
+    <t>Q' (m3/min)</t>
+  </si>
+  <si>
+    <t>Total System</t>
+  </si>
+  <si>
+    <t>2x DC-DC Convertor</t>
+  </si>
+  <si>
+    <t>Battery @ 200A</t>
+  </si>
+  <si>
+    <t>Battery @ 50A</t>
+  </si>
+  <si>
+    <t>9GA0412P3K01</t>
+  </si>
+  <si>
+    <t>Frame</t>
+  </si>
+  <si>
+    <t>40mm</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>9GAX0412P3S001</t>
+  </si>
+  <si>
+    <t>9S0612S4011</t>
+  </si>
+  <si>
+    <t>9S0612S409</t>
+  </si>
+  <si>
+    <t>60mm</t>
+  </si>
+  <si>
+    <t>SPL</t>
+  </si>
+  <si>
+    <t>9GA0612P7G01</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="16">
     <font>
@@ -1243,7 +1332,7 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1306,6 +1395,10 @@
     <xf numFmtId="48" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="5" builtinId="27"/>
@@ -1315,7 +1408,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3" xr:uid="{123B9C09-DBF4-C94E-B00F-92A47902B458}"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1343,36 +1436,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3051,6 +3114,533 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A580BCD-6644-FB4A-B224-B316B7ADE497}">
+  <dimension ref="A1:H37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="22" customHeight="1">
+      <c r="A3" s="56" t="s">
+        <v>308</v>
+      </c>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>317</v>
+      </c>
+      <c r="B4" t="s">
+        <v>318</v>
+      </c>
+      <c r="C4" t="s">
+        <v>319</v>
+      </c>
+      <c r="D4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="8">
+        <v>720</v>
+      </c>
+      <c r="B5" s="54">
+        <v>0.97</v>
+      </c>
+      <c r="C5" s="8">
+        <f>A5/B5</f>
+        <v>742.26804123711338</v>
+      </c>
+      <c r="D5" s="8">
+        <f xml:space="preserve"> CEILING(C5-A5,1)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>309</v>
+      </c>
+      <c r="B7" t="s">
+        <v>311</v>
+      </c>
+      <c r="C7" t="s">
+        <v>321</v>
+      </c>
+      <c r="D7" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="8">
+        <f>D$5</f>
+        <v>23</v>
+      </c>
+      <c r="B8">
+        <v>30</v>
+      </c>
+      <c r="C8" s="57">
+        <f>A8/20/B8</f>
+        <v>3.833333333333333E-2</v>
+      </c>
+      <c r="D8" s="57">
+        <f>C8*2</f>
+        <v>7.6666666666666661E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="8">
+        <f>D5</f>
+        <v>23</v>
+      </c>
+      <c r="B9">
+        <v>20</v>
+      </c>
+      <c r="C9" s="57">
+        <f>A9/20/B9</f>
+        <v>5.7499999999999996E-2</v>
+      </c>
+      <c r="D9" s="57">
+        <f>C9*2</f>
+        <v>0.11499999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="8">
+        <v>23</v>
+      </c>
+      <c r="B10">
+        <v>21</v>
+      </c>
+      <c r="C10" s="57">
+        <f>A10/20/B10</f>
+        <v>5.4761904761904755E-2</v>
+      </c>
+      <c r="D10" s="57">
+        <f>C10*2</f>
+        <v>0.10952380952380951</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="56" t="s">
+        <v>315</v>
+      </c>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>317</v>
+      </c>
+      <c r="B13" t="s">
+        <v>318</v>
+      </c>
+      <c r="C13" t="s">
+        <v>319</v>
+      </c>
+      <c r="D13" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="8">
+        <v>2480</v>
+      </c>
+      <c r="B14" s="54">
+        <v>0.9</v>
+      </c>
+      <c r="C14" s="8">
+        <f>A14/B14</f>
+        <v>2755.5555555555557</v>
+      </c>
+      <c r="D14" s="8">
+        <f xml:space="preserve"> CEILING(C14-A14,1)</f>
+        <v>276</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="8">
+        <f>50*12.8</f>
+        <v>640</v>
+      </c>
+      <c r="B15" s="54">
+        <v>0.9</v>
+      </c>
+      <c r="C15" s="8">
+        <f>A15/B15</f>
+        <v>711.11111111111109</v>
+      </c>
+      <c r="D15" s="8">
+        <f xml:space="preserve"> CEILING(C15-A15,1)</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>309</v>
+      </c>
+      <c r="B17" t="s">
+        <v>311</v>
+      </c>
+      <c r="C17" t="s">
+        <v>312</v>
+      </c>
+      <c r="D17" t="s">
+        <v>316</v>
+      </c>
+      <c r="E17" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="8">
+        <f>D$14</f>
+        <v>276</v>
+      </c>
+      <c r="B18">
+        <v>30</v>
+      </c>
+      <c r="C18" s="57">
+        <f>A18/20/B18</f>
+        <v>0.46</v>
+      </c>
+      <c r="D18" s="9">
+        <f>C18*1.5</f>
+        <v>0.69000000000000006</v>
+      </c>
+      <c r="E18" s="9">
+        <f>C18*2</f>
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="8">
+        <f t="shared" ref="A19:A20" si="0">D$14</f>
+        <v>276</v>
+      </c>
+      <c r="B19">
+        <v>40</v>
+      </c>
+      <c r="C19" s="57">
+        <f>A19/20/B19</f>
+        <v>0.34500000000000003</v>
+      </c>
+      <c r="D19" s="9">
+        <f>C19*1.5</f>
+        <v>0.51750000000000007</v>
+      </c>
+      <c r="E19" s="9">
+        <f>C19*2</f>
+        <v>0.69000000000000006</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="8">
+        <f t="shared" si="0"/>
+        <v>276</v>
+      </c>
+      <c r="B20">
+        <v>50</v>
+      </c>
+      <c r="C20" s="57">
+        <f>A20/20/B20</f>
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="D20" s="9">
+        <f>C20*1.5</f>
+        <v>0.41400000000000003</v>
+      </c>
+      <c r="E20" s="9">
+        <f>C20*2</f>
+        <v>0.55200000000000005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="56" t="s">
+        <v>322</v>
+      </c>
+      <c r="B22" s="40"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>323</v>
+      </c>
+      <c r="B23">
+        <f>A8*2</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>324</v>
+      </c>
+      <c r="B24" s="8">
+        <f>D14</f>
+        <v>276</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>325</v>
+      </c>
+      <c r="B25" s="8">
+        <f>D15</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="B26">
+        <f>SUM(B23:B25)</f>
+        <v>394</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>309</v>
+      </c>
+      <c r="B28" t="s">
+        <v>311</v>
+      </c>
+      <c r="C28" t="s">
+        <v>312</v>
+      </c>
+      <c r="D28" t="s">
+        <v>316</v>
+      </c>
+      <c r="E28" t="s">
+        <v>314</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+      <c r="G28">
+        <v>3</v>
+      </c>
+      <c r="H28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="8">
+        <f>B26</f>
+        <v>394</v>
+      </c>
+      <c r="B29">
+        <v>30</v>
+      </c>
+      <c r="C29" s="57">
+        <f>A29/20/B29</f>
+        <v>0.65666666666666662</v>
+      </c>
+      <c r="D29" s="9">
+        <f>C29*1.5</f>
+        <v>0.98499999999999988</v>
+      </c>
+      <c r="E29" s="9">
+        <f>C29*2</f>
+        <v>1.3133333333333332</v>
+      </c>
+      <c r="F29" s="9">
+        <f>$E29/F28</f>
+        <v>0.65666666666666662</v>
+      </c>
+      <c r="G29" s="9">
+        <f t="shared" ref="G29:H29" si="1">$E29/G28</f>
+        <v>0.43777777777777777</v>
+      </c>
+      <c r="H29" s="9">
+        <f t="shared" si="1"/>
+        <v>0.32833333333333331</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="B32" t="s">
+        <v>327</v>
+      </c>
+      <c r="C32" t="s">
+        <v>313</v>
+      </c>
+      <c r="D32" t="s">
+        <v>2</v>
+      </c>
+      <c r="E32" t="s">
+        <v>334</v>
+      </c>
+      <c r="F32" t="s">
+        <v>329</v>
+      </c>
+      <c r="G32" t="s">
+        <v>313</v>
+      </c>
+      <c r="H32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>326</v>
+      </c>
+      <c r="B33" t="s">
+        <v>328</v>
+      </c>
+      <c r="C33">
+        <v>0.81</v>
+      </c>
+      <c r="D33">
+        <v>35.5</v>
+      </c>
+      <c r="E33">
+        <v>54</v>
+      </c>
+      <c r="F33">
+        <v>2</v>
+      </c>
+      <c r="G33">
+        <f>C33*F33</f>
+        <v>1.62</v>
+      </c>
+      <c r="H33">
+        <f>D33*F33</f>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>330</v>
+      </c>
+      <c r="B34" t="s">
+        <v>328</v>
+      </c>
+      <c r="C34">
+        <v>0.9</v>
+      </c>
+      <c r="D34">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="E34">
+        <v>64</v>
+      </c>
+      <c r="F34">
+        <v>2</v>
+      </c>
+      <c r="G34">
+        <f>C34*F34</f>
+        <v>1.8</v>
+      </c>
+      <c r="H34">
+        <f>D34*F34</f>
+        <v>79.599999999999994</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>331</v>
+      </c>
+      <c r="B35" t="s">
+        <v>333</v>
+      </c>
+      <c r="C35">
+        <v>0.7</v>
+      </c>
+      <c r="D35">
+        <v>26.9</v>
+      </c>
+      <c r="E35">
+        <v>31</v>
+      </c>
+      <c r="F35">
+        <v>2</v>
+      </c>
+      <c r="G35">
+        <f>C35*F35</f>
+        <v>1.4</v>
+      </c>
+      <c r="H35">
+        <f>D35*F35</f>
+        <v>53.8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" t="s">
+        <v>332</v>
+      </c>
+      <c r="B36" t="s">
+        <v>333</v>
+      </c>
+      <c r="C36">
+        <v>0.74</v>
+      </c>
+      <c r="D36">
+        <v>30.9</v>
+      </c>
+      <c r="E36">
+        <v>31</v>
+      </c>
+      <c r="F36">
+        <v>2</v>
+      </c>
+      <c r="G36">
+        <f>C36*F36</f>
+        <v>1.48</v>
+      </c>
+      <c r="H36">
+        <f>D36*F36</f>
+        <v>61.8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" t="s">
+        <v>335</v>
+      </c>
+      <c r="B37" t="s">
+        <v>333</v>
+      </c>
+      <c r="C37">
+        <v>0.68</v>
+      </c>
+      <c r="D37">
+        <v>31.55</v>
+      </c>
+      <c r="E37">
+        <v>38</v>
+      </c>
+      <c r="F37">
+        <v>2</v>
+      </c>
+      <c r="G37">
+        <f>C37*F37</f>
+        <v>1.36</v>
+      </c>
+      <c r="H37">
+        <f>D37*F37</f>
+        <v>63.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92100D95-D95B-A341-A18C-0ED78105334C}">
   <dimension ref="A1:G8"/>
@@ -6563,7 +7153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EE2BD0D-CC3C-9D49-98D7-7EF532213FDA}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -6887,14 +7477,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E5:L9">
-    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
-      <formula>E5&lt;=$B$12</formula>
+    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
+      <formula>E5&gt;$B$13</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
       <formula>E5&gt;$B$12</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
-      <formula>E5&gt;$B$13</formula>
+    <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
+      <formula>E5&lt;=$B$12</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>